<commit_message>
#51, EXM-47523: Use XMLUtilAccess to escape text.
</commit_message>
<xml_diff>
--- a/test-sample/EXM-47523/_sample#@.xlsx
+++ b/test-sample/EXM-47523/_sample#@.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="&quot;Name #&amp;2&quot;" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="&quot;Name #2&quot;" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">dsda@32_</t>
+    <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@#dfsad</t>
+    <t xml:space="preserve">b</t>
   </si>
 </sst>
 </file>
@@ -139,7 +133,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.89"/>
   </cols>
@@ -152,18 +146,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="dsda@32_"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>